<commit_message>
Saved tidy data as ".txt" files
</commit_message>
<xml_diff>
--- a/data/2020-10-19_field-seasons_survey-tidy-data-01.xlsx
+++ b/data/2020-10-19_field-seasons_survey-tidy-data-01.xlsx
@@ -645,7 +645,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -689,7 +689,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">

</xml_diff>